<commit_message>
updated with the latest
</commit_message>
<xml_diff>
--- a/asplos_18.xlsx
+++ b/asplos_18.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2031" documentId="11_F25DC773A252ABEACE02ECA5E39F7D7C5ADE589E" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{9D75FA1B-70C2-4420-9FB6-67AA434DCC57}"/>
+  <xr:revisionPtr revIDLastSave="2039" documentId="11_F25DC773A252ABEACE02ECA5E39F7D7C5ADE589E" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{974606AB-E4B5-4590-B339-30F8AC3CF2DF}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" firstSheet="13" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" firstSheet="14" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fig-postgresql-combined-use (2)" sheetId="31" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="225">
   <si>
     <t>Clang 6.0.0</t>
   </si>
@@ -731,6 +731,9 @@
   </si>
   <si>
     <t>Js_Ls</t>
+  </si>
+  <si>
+    <t>PostgreSQL-r</t>
   </si>
 </sst>
 </file>
@@ -30956,8 +30959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA11CC75-C6CA-4F4C-8FD1-11B9831EB089}">
   <dimension ref="A1:I164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124:XFD124"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -31975,45 +31978,105 @@
       <c r="A77" t="s">
         <v>217</v>
       </c>
+      <c r="B77" s="2">
+        <v>108820.90065</v>
+      </c>
+      <c r="C77" s="2">
+        <v>65588.486199999999</v>
+      </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>218</v>
       </c>
+      <c r="B78" s="2">
+        <v>37100.914250000002</v>
+      </c>
+      <c r="C78" s="2">
+        <v>15929.632449999999</v>
+      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>219</v>
       </c>
+      <c r="B79" s="2">
+        <v>188444.31450000001</v>
+      </c>
+      <c r="C79" s="2">
+        <v>187755.08705</v>
+      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>220</v>
       </c>
+      <c r="B80" s="2">
+        <v>563034.05530000001</v>
+      </c>
+      <c r="C80" s="2">
+        <v>729586.17575000005</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>164</v>
       </c>
+      <c r="B81" s="2">
+        <v>13754650.135849999</v>
+      </c>
+      <c r="C81" s="2">
+        <v>6346313.0857999995</v>
+      </c>
+      <c r="D81">
+        <f>B81/B82</f>
+        <v>4.6368426294371559E-2</v>
+      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>161</v>
       </c>
+      <c r="B82" s="2">
+        <v>296638278.13625002</v>
+      </c>
+      <c r="C82" s="2">
+        <v>278591770.82305002</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>160</v>
       </c>
+      <c r="B83" s="2">
+        <v>249029650.24184999</v>
+      </c>
+      <c r="C83" s="2">
+        <v>239468462.65625</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>221</v>
       </c>
+      <c r="B84" s="2">
+        <v>28324040.555</v>
+      </c>
+      <c r="C84" s="2">
+        <v>23554074.528549999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B85" s="2">
+        <v>431.85849999999999</v>
+      </c>
+      <c r="C85" s="2">
+        <v>400.31549999999999</v>
+      </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>61</v>
+        <v>224</v>
       </c>
       <c r="B90" t="s">
         <v>131</v>
@@ -32321,7 +32384,7 @@
         <v>2486650725.50281</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>221</v>
       </c>
@@ -32332,7 +32395,7 @@
         <v>49920902.113750003</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B130" s="2">
         <v>440.52</v>
       </c>
@@ -32340,7 +32403,7 @@
         <v>442.23500000000001</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>60</v>
       </c>
@@ -32351,44 +32414,104 @@
         <v>132</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B139" s="2">
+        <v>8737575.9550000001</v>
+      </c>
+      <c r="C139" s="2">
+        <v>7933801.6550000003</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B140" s="2">
+        <v>5865192.2800000003</v>
+      </c>
+      <c r="C140" s="2">
+        <v>5258963.26</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B141" s="2">
+        <v>3402177.4950000001</v>
+      </c>
+      <c r="C141" s="2">
+        <v>3887085.0649999999</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B142" s="2">
+        <v>14540766.880000001</v>
+      </c>
+      <c r="C142" s="2">
+        <v>15634365.789999999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B143" s="2">
+        <v>6333039173.9449997</v>
+      </c>
+      <c r="C143" s="2">
+        <v>5393129383.2849998</v>
+      </c>
+      <c r="D143">
+        <f>B143/B144</f>
+        <v>8.8506998675117132E-2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>161</v>
+      </c>
+      <c r="B144" s="2">
+        <v>71554106101.729904</v>
+      </c>
+      <c r="C144" s="2">
+        <v>71064630795.535004</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>160</v>
       </c>
+      <c r="B145" s="2">
+        <v>93528118073.720001</v>
+      </c>
+      <c r="C145" s="2">
+        <v>93503701386.619904</v>
+      </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>221</v>
+      </c>
+      <c r="B146" s="2">
+        <v>1256978851.73</v>
+      </c>
+      <c r="C146" s="2">
+        <v>1251484449.3099999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B147" s="2">
+        <v>1022.218</v>
+      </c>
+      <c r="C147" s="2">
+        <v>1014.6255</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.45">

</xml_diff>